<commit_message>
Validaciones y listas en archivo carga_masiva.xlsx
</commit_message>
<xml_diff>
--- a/static/file/carga_masiva.xlsx
+++ b/static/file/carga_masiva.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Libe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\liberalia_app\liberalia-app\static\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8A8ABB5-5057-4CD8-9F95-8808B2D026C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C8E55-C5F7-47FE-92CB-9E2063B432C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E23137C1-A7A0-4594-B862-11412BF4798A}"/>
   </bookViews>
@@ -370,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,12 +380,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF7B1E2D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor rgb="FF7B1E2D"/>
       </patternFill>
     </fill>
@@ -403,71 +397,262 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -508,36 +693,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{465C66AA-5E53-40CF-89B1-0D5772751103}" name="Tabla1" displayName="Tabla1" ref="A1:Z2" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{465C66AA-5E53-40CF-89B1-0D5772751103}" name="Tabla1" displayName="Tabla1" ref="A1:Z2" totalsRowShown="0" headerRowDxfId="27" dataDxfId="0">
   <tableColumns count="26">
-    <tableColumn id="1" xr3:uid="{7C784B33-88A0-416D-B458-604BCB4BA743}" name="Isbn" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{32ADA3A5-46D6-4247-8F33-0C49456461FE}" name="Ean" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{DF83E792-4DF6-4911-908E-4144B30EC61A}" name="Editorial"/>
-    <tableColumn id="4" xr3:uid="{4AD2648D-F707-4F77-91F7-EC9A52B60499}" name="Titulo"/>
-    <tableColumn id="5" xr3:uid="{38F2673B-324B-4DF9-961C-0110480FA904}" name="Subtitulo"/>
-    <tableColumn id="6" xr3:uid="{E6A7D40E-7D13-4AD9-B48E-26C92604381F}" name="Autor"/>
-    <tableColumn id="7" xr3:uid="{7CD24112-DA25-442C-8176-6A62AF91F594}" name="Autor Prologo"/>
-    <tableColumn id="8" xr3:uid="{3A985C05-6CD9-4AB5-94F1-3933BCAF4F05}" name="Traductor"/>
-    <tableColumn id="9" xr3:uid="{C990CBCF-1B6C-401E-9112-CD78CAB53DE2}" name="Ilustrador"/>
-    <tableColumn id="10" xr3:uid="{75DE1AEF-73BB-4983-9B02-DA644658547C}" name="Tipo Tapa"/>
-    <tableColumn id="11" xr3:uid="{77C5117F-E400-48F0-87EF-32CE99C59015}" name="Numero Paginas" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{90F72465-0160-4F26-9967-92A9AA512AF8}" name="Alto Cm" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{1BA043F0-5CB4-48DC-A32D-CDE52E2CBA4C}" name="Ancho Cm" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{F2CB0F23-BFC1-4690-B84D-282B74EDD442}" name="Grosor Cm" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{7D5F7C1E-17E6-4A94-AD8C-1288C4DDE7A0}" name="Peso Gr" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{2955DEEA-DF35-4DD0-A03B-CD1AB3EA93CE}" name="Idioma Original" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{A28C6831-8FE5-45EC-8070-DFDBC4EAB277}" name="Numero Edicion" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{CF26DB9A-3DBC-4956-8488-7C02DB9174C1}" name="Fecha Edicion"/>
-    <tableColumn id="19" xr3:uid="{3F388524-D312-4140-8114-DB921BFC87E9}" name="Pais Edicion"/>
-    <tableColumn id="20" xr3:uid="{AEDC4012-08AC-4821-88CC-91D1CF2D202B}" name="Numero Impresion" dataDxfId="3"/>
-    <tableColumn id="21" xr3:uid="{779BA726-F596-4954-B7F1-DF0A16BA60FB}" name="Tematica"/>
-    <tableColumn id="22" xr3:uid="{FFD8EC28-19DE-4278-B082-3C7D264CFF83}" name="Precio" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{F79C06B3-87D9-4009-8276-CA958837A1C5}" name="Moneda" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{287EDACE-7356-4A86-925A-2844327FE969}" name="Descuento Distribuidor" dataCellStyle="Porcentaje"/>
-    <tableColumn id="25" xr3:uid="{392FDB95-2080-47E1-8D25-A989EF738499}" name="Resumen Libro"/>
-    <tableColumn id="26" xr3:uid="{180FA28D-905C-4762-A814-0EE31B5AF325}" name="Rango Etario" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{7C784B33-88A0-416D-B458-604BCB4BA743}" name="Isbn" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{32ADA3A5-46D6-4247-8F33-0C49456461FE}" name="Ean" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{DF83E792-4DF6-4911-908E-4144B30EC61A}" name="Editorial" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{4AD2648D-F707-4F77-91F7-EC9A52B60499}" name="Titulo" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{38F2673B-324B-4DF9-961C-0110480FA904}" name="Subtitulo" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{E6A7D40E-7D13-4AD9-B48E-26C92604381F}" name="Autor" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{7CD24112-DA25-442C-8176-6A62AF91F594}" name="Autor Prologo" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{3A985C05-6CD9-4AB5-94F1-3933BCAF4F05}" name="Traductor" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{C990CBCF-1B6C-401E-9112-CD78CAB53DE2}" name="Ilustrador" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{75DE1AEF-73BB-4983-9B02-DA644658547C}" name="Tipo Tapa" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{77C5117F-E400-48F0-87EF-32CE99C59015}" name="Numero Paginas" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{90F72465-0160-4F26-9967-92A9AA512AF8}" name="Alto Cm" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{1BA043F0-5CB4-48DC-A32D-CDE52E2CBA4C}" name="Ancho Cm" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{F2CB0F23-BFC1-4690-B84D-282B74EDD442}" name="Grosor Cm" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{7D5F7C1E-17E6-4A94-AD8C-1288C4DDE7A0}" name="Peso Gr" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{2955DEEA-DF35-4DD0-A03B-CD1AB3EA93CE}" name="Idioma Original" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{A28C6831-8FE5-45EC-8070-DFDBC4EAB277}" name="Numero Edicion" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{CF26DB9A-3DBC-4956-8488-7C02DB9174C1}" name="Fecha Edicion" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{3F388524-D312-4140-8114-DB921BFC87E9}" name="Pais Edicion" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{AEDC4012-08AC-4821-88CC-91D1CF2D202B}" name="Numero Impresion" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{779BA726-F596-4954-B7F1-DF0A16BA60FB}" name="Tematica" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{FFD8EC28-19DE-4278-B082-3C7D264CFF83}" name="Precio" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{F79C06B3-87D9-4009-8276-CA958837A1C5}" name="Moneda" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{287EDACE-7356-4A86-925A-2844327FE969}" name="Descuento Distribuidor" dataDxfId="3" dataCellStyle="Porcentaje"/>
+    <tableColumn id="25" xr3:uid="{392FDB95-2080-47E1-8D25-A989EF738499}" name="Resumen Libro" dataDxfId="2"/>
+    <tableColumn id="26" xr3:uid="{180FA28D-905C-4762-A814-0EE31B5AF325}" name="Rango Etario" dataDxfId="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -861,7 +1046,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +1083,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -907,19 +1092,19 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -928,16 +1113,16 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -952,10 +1137,10 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="12" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
@@ -970,26 +1155,26 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="5"/>
-      <c r="T2" s="3"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="7"/>
-      <c r="Z2" s="8"/>
+    <row r="2" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="8"/>
+      <c r="T2" s="5"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="10"/>
+      <c r="Z2" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="13">
@@ -1088,65 +1273,65 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="9" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="9" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="9" t="s">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="9"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="3" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>